<commit_message>
Finished first draft of chapter 2
</commit_message>
<xml_diff>
--- a/writeup/results/parse-lengths.xlsx
+++ b/writeup/results/parse-lengths.xlsx
@@ -5842,6 +5842,146 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>evalvsdictionary!$C$5:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>evalvsdictionary!$D$5:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>572.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2392.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17905.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84058.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>595537.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.38067E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.281865E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4402284E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4402284E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4402284E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>evalvsdictionary!$C$5:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>evalvsdictionary!$D$5:$D$16</c:f>
@@ -5934,6 +6074,7 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6030,6 +6171,7 @@
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -6119,7 +6261,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9202295" cy="5610902"/>
+    <xdr:ext cx="9191885" cy="5610902"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -15651,6 +15793,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>